<commit_message>
map CapitalTransferInformation from Excel input
</commit_message>
<xml_diff>
--- a/adapter-excel/src/test/resources/retirement-fund-test-data_de.xlsx
+++ b/adapter-excel/src/test/resources/retirement-fund-test-data_de.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Eintritte" sheetId="1" r:id="rId1"/>
-    <sheet name="Austritte" sheetId="2" r:id="rId2"/>
+    <sheet name="Austritte" sheetId="1" r:id="rId1"/>
+    <sheet name="Eintritte" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -155,7 +155,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>AHV-Nummer</t>
   </si>
@@ -224,6 +224,9 @@
   </si>
   <si>
     <t>Austrittsinformationen</t>
+  </si>
+  <si>
+    <t>Zahlungszweck</t>
   </si>
 </sst>
 </file>
@@ -623,8 +626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1128,8 +1131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1226,13 +1229,27 @@
       <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>

</xml_diff>

<commit_message>
adjust Excel columns after PO feedback
- isrReference not relevant for MVP
- reference moved to existing attribute 'internalReferenz' on jobInfo
</commit_message>
<xml_diff>
--- a/adapter-excel/src/test/resources/retirement-fund-test-data_de.xlsx
+++ b/adapter-excel/src/test/resources/retirement-fund-test-data_de.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="390" yWindow="5970" windowWidth="30960" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Austritte" sheetId="1" r:id="rId1"/>
@@ -72,90 +72,8 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Autor</author>
-  </authors>
-  <commentList>
-    <comment ref="A2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t>Autor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-http://rolfa.ch/ahv</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t>Autor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-https://www.uid.admin.ch/Search.aspx</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t>Autor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-https://www.six-interbank-clearing.com/de/home/standardization/iban/inquiry-iban.html</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>AHV-Nummer</t>
   </si>
@@ -163,9 +81,6 @@
     <t>Datum</t>
   </si>
   <si>
-    <t xml:space="preserve">Zahlungszweck </t>
-  </si>
-  <si>
     <t>UID der VE</t>
   </si>
   <si>
@@ -187,9 +102,6 @@
     <t>IBAN</t>
   </si>
   <si>
-    <t>ESR Referenznummer</t>
-  </si>
-  <si>
     <t>CHE-109.740.084</t>
   </si>
   <si>
@@ -208,9 +120,6 @@
     <t>CHE-223.471.073</t>
   </si>
   <si>
-    <t>Perspectiva Sammelstiftung für berufliche Vorsorge</t>
-  </si>
-  <si>
     <t>7569678192446</t>
   </si>
   <si>
@@ -226,7 +135,19 @@
     <t>Austrittsinformationen</t>
   </si>
   <si>
-    <t>Zahlungszweck</t>
+    <t>Referenz</t>
+  </si>
+  <si>
+    <t>our-ref-1</t>
+  </si>
+  <si>
+    <t>our-ref-2</t>
+  </si>
+  <si>
+    <t>our-ref-55</t>
+  </si>
+  <si>
+    <t>our-ref-56</t>
   </si>
 </sst>
 </file>
@@ -627,7 +548,7 @@
   <dimension ref="A1:D145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,7 +560,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -653,38 +574,38 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B3" s="4">
         <v>43252</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B4" s="4">
         <v>43328</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1128,8 +1049,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K98"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
@@ -1137,17 +1058,21 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="21.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="67.140625" customWidth="1"/>
-    <col min="5" max="9" width="21.5703125" customWidth="1"/>
-    <col min="10" max="10" width="24" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" customWidth="1"/>
+    <col min="5" max="5" width="66.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="21.5703125" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" customWidth="1"/>
     <col min="11" max="11" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1158,9 +1083,8 @@
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-    </row>
-    <row r="2" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:10" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1168,123 +1092,118 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" s="4">
         <v>43101</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B4" s="4">
         <v>43327</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
@@ -1506,39 +1425,11 @@
     <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" s="5"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B90" s="5"/>
-    </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B91" s="5"/>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B92" s="5"/>
-    </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B93" s="5"/>
-    </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B94" s="5"/>
-    </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B95" s="5"/>
-    </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B96" s="5"/>
-    </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B97" s="5"/>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B98" s="5"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>